<commit_message>
Added Test Case no34
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5978EBD3-7FB4-4E9B-9AA0-359E4C656D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27099A4C-1EB9-4E9F-A789-75EFD2342685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="108">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_034</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
+    <t>Leverage</t>
+  </si>
+  <si>
+    <t>Margin Type</t>
+  </si>
+  <si>
+    <t>CROSSED</t>
   </si>
 </sst>
 </file>
@@ -421,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -437,6 +449,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -889,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,13 +918,15 @@
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -935,34 +952,40 @@
         <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -984,11 +1007,13 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1008,11 +1033,13 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1032,11 +1059,13 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1056,11 +1085,13 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1082,11 +1113,13 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1106,11 +1139,13 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1132,11 +1167,13 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1162,11 +1199,13 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1192,11 +1231,13 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -1214,23 +1255,25 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2">
-        <v>1</v>
-      </c>
+      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1251,20 +1294,22 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
+      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -1282,23 +1327,25 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1316,23 +1363,25 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
+      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -1350,23 +1399,25 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
+      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1384,21 +1435,23 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
-      <c r="Q16" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
@@ -1417,23 +1470,25 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7">
-        <v>1</v>
-      </c>
+      <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+      <c r="N17" s="7">
+        <v>1</v>
+      </c>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-      <c r="Q17" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
@@ -1446,14 +1501,29 @@
       <c r="F18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O18" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="H18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="9">
+        <v>25</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1</v>
+      </c>
+      <c r="S18" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F19" s="8"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added test case number 35
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27099A4C-1EB9-4E9F-A789-75EFD2342685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FE7A52-1D26-4AAE-9F1B-3F21D9998BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="109">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -341,12 +341,18 @@
   </si>
   <si>
     <t>CROSSED</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -415,25 +421,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -448,8 +441,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -906,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1482,8 +1480,12 @@
       </c>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="Q17" s="7">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7">
+        <v>1</v>
+      </c>
       <c r="S17" s="7" t="b">
         <v>0</v>
       </c>
@@ -1504,7 +1506,7 @@
       <c r="H18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <v>25</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -1519,12 +1521,50 @@
       <c r="Q18" s="2">
         <v>1</v>
       </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
       <c r="S18" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="F19" s="8"/>
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="8">
+        <v>25</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>
@@ -1537,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
-  <dimension ref="A1:AP8"/>
+  <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2205,6 +2245,50 @@
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
     </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added steps for test case 28
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FE7A52-1D26-4AAE-9F1B-3F21D9998BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B843ED74-5CA3-4F6C-B469-D3C6C5EA5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_035</t>
+  </si>
+  <si>
+    <t>twap_bot</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>1m</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
-  <dimension ref="A1:AP9"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1589,7 +1598,7 @@
     <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1618,106 +1627,112 @@
         <v>43</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -1744,62 +1759,64 @@
         <v>1</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="2">
+      <c r="N2" s="2">
         <v>20</v>
       </c>
-      <c r="M2" s="2">
+      <c r="O2" s="2">
         <v>50</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2">
         <v>1E-3</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2">
         <v>3000</v>
       </c>
-      <c r="T2" s="2">
+      <c r="V2" s="2">
         <v>4000</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="2">
-        <v>1</v>
-      </c>
+      <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
+      <c r="AK2" s="2">
+        <v>1</v>
+      </c>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
-      <c r="AN2" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
-      <c r="AP2" s="2" t="s">
+      <c r="AP2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>77</v>
       </c>
@@ -1826,60 +1843,62 @@
         <v>1</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>20</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>50</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2">
         <v>1E-3</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2">
         <v>3100</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>3900</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="2">
-        <v>1</v>
-      </c>
+      <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
+      <c r="AK3" s="2">
+        <v>1</v>
+      </c>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
-      <c r="AN3" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
@@ -1925,33 +1944,35 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="2" t="s">
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AG4" s="2">
         <v>0.1</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AH4" s="2">
         <v>3000</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AI4" s="2">
         <v>4000</v>
       </c>
-      <c r="AH4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AJ4" s="2">
+        <v>1</v>
+      </c>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
-      <c r="AN4" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -1997,33 +2018,35 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="2" t="s">
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AG5" s="2">
         <v>0.1</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AH5" s="2">
         <v>3000</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AI5" s="2">
         <v>4000</v>
       </c>
-      <c r="AH5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AJ5" s="2">
+        <v>1</v>
+      </c>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
-      <c r="AN5" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
-      <c r="AP5" s="2"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -2044,13 +2067,17 @@
         <v>72</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1234</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -2069,33 +2096,37 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="2" t="s">
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AG6" s="2">
         <v>0.1</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AH6" s="2">
         <v>3000</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AI6" s="2">
         <v>4000</v>
       </c>
-      <c r="AH6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
+      <c r="AJ6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>1</v>
+      </c>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
-      <c r="AN6" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>83</v>
       </c>
@@ -2141,33 +2172,35 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="2" t="s">
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AG7" s="2">
         <v>0.1</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AH7" s="2">
         <v>3000</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AI7" s="2">
         <v>4000</v>
       </c>
-      <c r="AH7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AJ7" s="2">
+        <v>1</v>
+      </c>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
-      <c r="AN7" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>84</v>
       </c>
@@ -2213,39 +2246,41 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="2" t="s">
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AG8" s="2">
         <v>0.1</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AH8" s="2">
         <v>3000</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AI8" s="2">
         <v>4000</v>
       </c>
-      <c r="AH8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="2">
+      <c r="AJ8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="2">
         <v>200</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="AL8" s="2">
         <v>10</v>
       </c>
-      <c r="AK8" s="2" t="s">
+      <c r="AM8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="AP8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2255,8 +2290,8 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2275,21 +2310,24 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="9"/>
       <c r="AH9" s="10"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
-      <c r="AM9" s="6"/>
-      <c r="AN9" s="6"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New steps in 28th Test case
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B843ED74-5CA3-4F6C-B469-D3C6C5EA5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0137F1-B5AA-4E49-B480-66CD6CDB585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="113">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>1m</t>
+  </si>
+  <si>
+    <t>TSIDE</t>
   </si>
 </sst>
 </file>
@@ -1586,10 +1589,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
-  <dimension ref="A1:AR9"/>
+  <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1598,7 +1601,7 @@
     <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1630,109 +1633,112 @@
         <v>110</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -1761,62 +1767,63 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>20</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>50</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
         <v>1E-3</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2">
+      <c r="U2" s="2"/>
+      <c r="V2" s="2">
         <v>3000</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>4000</v>
       </c>
-      <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
-      <c r="AK2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2">
+        <v>1</v>
+      </c>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
-      <c r="AP2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2" t="s">
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>77</v>
       </c>
@@ -1845,60 +1852,61 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>20</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>50</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
         <v>1E-3</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="2">
+      <c r="U3" s="2"/>
+      <c r="V3" s="2">
         <v>3100</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
         <v>3900</v>
       </c>
-      <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
-      <c r="AK3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2">
+        <v>1</v>
+      </c>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR3" s="2"/>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
@@ -1946,33 +1954,34 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
-      <c r="AF4" s="2" t="s">
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AH4" s="2">
         <v>0.1</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AI4" s="2">
         <v>3000</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AJ4" s="2">
         <v>4000</v>
       </c>
-      <c r="AJ4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="2"/>
+      <c r="AK4" s="2">
+        <v>1</v>
+      </c>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
-      <c r="AP4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR4" s="2"/>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS4" s="2"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2020,33 +2029,34 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
-      <c r="AF5" s="2" t="s">
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AH5" s="2">
         <v>0.1</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="AI5" s="2">
         <v>3000</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AJ5" s="2">
         <v>4000</v>
       </c>
-      <c r="AJ5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="2"/>
+      <c r="AK5" s="2">
+        <v>1</v>
+      </c>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
-      <c r="AP5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR5" s="2"/>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS5" s="2"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
@@ -2075,10 +2085,12 @@
       <c r="J6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="2">
         <v>1234</v>
       </c>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2098,35 +2110,36 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
-      <c r="AF6" s="2" t="s">
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AH6" s="2">
         <v>0.1</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AI6" s="2">
         <v>3000</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AJ6" s="2">
         <v>4000</v>
       </c>
-      <c r="AJ6" s="2">
-        <v>1</v>
-      </c>
       <c r="AK6" s="2">
         <v>1</v>
       </c>
-      <c r="AL6" s="2"/>
+      <c r="AL6" s="2">
+        <v>1</v>
+      </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR6" s="2"/>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS6" s="2"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>83</v>
       </c>
@@ -2174,33 +2187,34 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
-      <c r="AF7" s="2" t="s">
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AH7" s="2">
         <v>0.1</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AI7" s="2">
         <v>3000</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AJ7" s="2">
         <v>4000</v>
       </c>
-      <c r="AJ7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK7" s="2"/>
+      <c r="AK7" s="2">
+        <v>1</v>
+      </c>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR7" s="2"/>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS7" s="2"/>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>84</v>
       </c>
@@ -2248,39 +2262,40 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
-      <c r="AF8" s="2" t="s">
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AH8" s="2">
         <v>0.1</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AI8" s="2">
         <v>3000</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AJ8" s="2">
         <v>4000</v>
       </c>
-      <c r="AJ8" s="2">
-        <v>1</v>
-      </c>
       <c r="AK8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="2">
         <v>200</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="AM8" s="2">
         <v>10</v>
       </c>
-      <c r="AM8" s="2" t="s">
+      <c r="AN8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
-      <c r="AP8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="AR8" s="2"/>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="AS8" s="2"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2292,7 +2307,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2312,19 +2327,20 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
-      <c r="AF9" s="4"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="10"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="9"/>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="10"/>
-      <c r="AK9" s="2"/>
+      <c r="AK9" s="10"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
-      <c r="AO9" s="6"/>
+      <c r="AO9" s="2"/>
       <c r="AP9" s="6"/>
-      <c r="AQ9" s="2"/>
+      <c r="AQ9" s="6"/>
       <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Twap test case number 28 and 29
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0137F1-B5AA-4E49-B480-66CD6CDB585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DDE9D7-EA0E-4715-92EB-C63416AB6723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1591,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1959,7 +1959,7 @@
         <v>33</v>
       </c>
       <c r="AH4" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AI4" s="2">
         <v>3000</v>
@@ -2034,7 +2034,7 @@
         <v>78</v>
       </c>
       <c r="AH5" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="2">
         <v>3000</v>
@@ -2086,11 +2086,9 @@
         <v>111</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1234</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2112,7 +2110,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="AH6" s="2">
         <v>0.1</v>
@@ -2160,13 +2158,17 @@
         <v>72</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2203,7 +2205,9 @@
       <c r="AK7" s="2">
         <v>1</v>
       </c>
-      <c r="AL7" s="2"/>
+      <c r="AL7" s="2">
+        <v>1</v>
+      </c>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>

</xml_diff>

<commit_message>
Added new account details into test data sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8567D0-1BD5-4735-9A18-B7B042A2EC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4BC02-0875-4679-9190-0DC65C3E0FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -100,9 +100,6 @@
     <t>QA_TestCase_Auto_NitroX_009</t>
   </si>
   <si>
-    <t>Trader01@Tinyex</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_010</t>
   </si>
   <si>
@@ -362,6 +359,12 @@
   </si>
   <si>
     <t>LTC/USDT Perpetual USDT</t>
+  </si>
+  <si>
+    <t>Automation_Bot@Tinyex</t>
+  </si>
+  <si>
+    <t>Automation_OrderBook@Tinyex</t>
   </si>
 </sst>
 </file>
@@ -825,16 +828,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -845,16 +848,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -866,19 +869,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="6" t="b">
@@ -887,19 +890,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="b">
@@ -922,14 +925,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" bestFit="1" customWidth="1"/>
@@ -959,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -968,10 +971,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>11</v>
@@ -1141,7 +1144,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1163,13 +1166,13 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1191,16 +1194,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>2</v>
@@ -1223,16 +1226,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>2</v>
@@ -1255,16 +1258,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2</v>
@@ -1274,7 +1277,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1291,16 +1294,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
@@ -1327,16 +1330,16 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
@@ -1346,7 +1349,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1363,16 +1366,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2</v>
@@ -1382,7 +1385,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1399,16 +1402,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
@@ -1418,7 +1421,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1435,16 +1438,16 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>2</v>
@@ -1454,7 +1457,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1469,16 +1472,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>27</v>
+      <c r="C17" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>2</v>
@@ -1489,7 +1492,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -1510,28 +1513,28 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" s="8">
         <v>25</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" s="2">
         <v>1</v>
@@ -1548,28 +1551,28 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I19" s="8">
         <v>25</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="2">
         <v>1</v>
@@ -1586,28 +1589,28 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I20" s="8">
         <v>25</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N20" s="2">
         <v>1</v>
@@ -1626,8 +1629,12 @@
       <c r="B34" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{FD3BAB66-20EF-4340-AAA8-8DC0A130EAC4}"/>
+    <hyperlink ref="C8:C17" r:id="rId2" display="Automation_OrderBook@Tinyex" xr:uid="{AA208809-3E4A-405C-823F-E40F535E6767}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1635,14 +1642,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
     <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.90625" bestFit="1" customWidth="1"/>
@@ -1668,106 +1675,106 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AH1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="AL1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AO1" s="2" t="s">
         <v>17</v>
@@ -1779,46 +1786,46 @@
         <v>3</v>
       </c>
       <c r="AR1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2">
         <v>20</v>
@@ -1831,7 +1838,7 @@
         <v>1E-3</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -1848,12 +1855,12 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
@@ -1873,43 +1880,43 @@
       </c>
       <c r="AR2" s="2"/>
       <c r="AS2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O3" s="2">
         <v>20</v>
@@ -1922,7 +1929,7 @@
         <v>1E-3</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -1939,7 +1946,7 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
@@ -1965,26 +1972,26 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
@@ -2013,7 +2020,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH4" s="2">
         <v>1</v>
@@ -2040,26 +2047,26 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="2">
         <v>1</v>
@@ -2088,7 +2095,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH5" s="2">
         <v>1</v>
@@ -2115,35 +2122,35 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -2167,7 +2174,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH6" s="2">
         <v>0.1</v>
@@ -2196,35 +2203,35 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2248,7 +2255,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH7" s="2">
         <v>0.1</v>
@@ -2277,26 +2284,26 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -2325,7 +2332,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH8" s="2">
         <v>0.1</v>
@@ -2346,7 +2353,7 @@
         <v>10</v>
       </c>
       <c r="AN8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
@@ -2404,7 +2411,11 @@
       <c r="AS9" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8D3AFE74-93CB-4B51-8F82-1315FE188304}"/>
+    <hyperlink ref="C3:C8" r:id="rId2" display="Automation_Bot@Tinyex" xr:uid="{CDDD482D-E149-413F-BF8F-1FA68756936E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Bots Feature file and Steps with new Trading account
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4BC02-0875-4679-9190-0DC65C3E0FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3015A245-9A53-4137-80C4-013B338F32B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -447,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -471,6 +471,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -925,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1643,15 +1644,29 @@
   <dimension ref="A1:AS9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.08984375" customWidth="1"/>
+    <col min="24" max="24" width="14.7265625" customWidth="1"/>
+    <col min="25" max="25" width="23.7265625" customWidth="1"/>
+    <col min="26" max="26" width="8.7265625" customWidth="1"/>
+    <col min="27" max="27" width="19.1796875" customWidth="1"/>
+    <col min="28" max="28" width="14.08984375" customWidth="1"/>
+    <col min="29" max="29" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1834,8 +1849,8 @@
         <v>50</v>
       </c>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2">
-        <v>1E-3</v>
+      <c r="R2" s="11">
+        <v>0.1</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>73</v>
@@ -1925,8 +1940,8 @@
         <v>50</v>
       </c>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2">
-        <v>1E-3</v>
+      <c r="R3" s="11">
+        <v>0.1</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>73</v>
@@ -2037,7 +2052,9 @@
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
+      <c r="AO4" s="2">
+        <v>1</v>
+      </c>
       <c r="AP4" s="2"/>
       <c r="AQ4" s="2" t="b">
         <v>0</v>
@@ -2112,7 +2129,9 @@
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
+      <c r="AO5" s="2">
+        <v>1</v>
+      </c>
       <c r="AP5" s="2"/>
       <c r="AQ5" s="2" t="b">
         <v>0</v>
@@ -2193,7 +2212,9 @@
       </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
+      <c r="AO6" s="2">
+        <v>1</v>
+      </c>
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2" t="b">
         <v>0</v>
@@ -2274,7 +2295,9 @@
       </c>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
+      <c r="AO7" s="2">
+        <v>1</v>
+      </c>
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2" t="b">
         <v>0</v>
@@ -2355,7 +2378,9 @@
       <c r="AN8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AO8" s="2"/>
+      <c r="AO8" s="2">
+        <v>1</v>
+      </c>
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2" t="b">
         <v>0</v>
@@ -2412,10 +2437,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{8D3AFE74-93CB-4B51-8F82-1315FE188304}"/>
-    <hyperlink ref="C3:C8" r:id="rId2" display="Automation_Bot@Tinyex" xr:uid="{CDDD482D-E149-413F-BF8F-1FA68756936E}"/>
+    <hyperlink ref="C3:C8" r:id="rId1" display="Automation_Bot@Tinyex" xr:uid="{CDDD482D-E149-413F-BF8F-1FA68756936E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test case 36 added Scenario and Modified the Bot Feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3015A245-9A53-4137-80C4-013B338F32B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3BAB8C-4757-4E88-99A3-5EF5BAE888C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -358,13 +358,16 @@
     <t>QA_TestCase_Auto_NitroX_036</t>
   </si>
   <si>
-    <t>LTC/USDT Perpetual USDT</t>
-  </si>
-  <si>
     <t>Automation_Bot@Tinyex</t>
   </si>
   <si>
     <t>Automation_OrderBook@Tinyex</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_036_01</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_037</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,13 +400,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -447,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -472,6 +488,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -811,39 +828,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878D5118-86AA-443A-B8A4-36B93CD796C0}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.7265625" customWidth="1"/>
     <col min="2" max="2" width="48.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
     <col min="7" max="7" width="66.1796875" customWidth="1"/>
+    <col min="8" max="26" width="8.7265625" customWidth="1"/>
+    <col min="27" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -924,84 +948,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
     <col min="3" max="3" width="28.81640625" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.7265625" customWidth="1"/>
     <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.7265625" customWidth="1"/>
+    <col min="17" max="17" width="34.1796875" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" customWidth="1"/>
+    <col min="19" max="19" width="8.08984375" customWidth="1"/>
+    <col min="20" max="26" width="8.7265625" customWidth="1"/>
+    <col min="27" max="16379" width="8.7265625" hidden="1"/>
+    <col min="16380" max="16380" width="25.26953125" hidden="1"/>
+    <col min="16381" max="16381" width="16.90625" hidden="1"/>
+    <col min="16382" max="16382" width="26.6328125" hidden="1"/>
+    <col min="16383" max="16383" width="15.453125" hidden="1"/>
+    <col min="16384" max="16384" width="2.90625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1145,7 +1182,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1173,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1201,7 +1238,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -1233,7 +1270,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -1265,7 +1302,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
@@ -1301,7 +1338,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>29</v>
@@ -1337,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
@@ -1373,7 +1410,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -1409,7 +1446,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -1445,7 +1482,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -1479,7 +1516,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>29</v>
@@ -1599,7 +1636,7 @@
         <v>101</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>103</v>
@@ -1623,6 +1660,82 @@
         <v>1</v>
       </c>
       <c r="S20" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" s="8">
+        <v>25</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+      <c r="S21" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" s="8">
+        <v>25</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1</v>
+      </c>
+      <c r="S22" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1641,25 +1754,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
-  <dimension ref="A1:AS9"/>
+  <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
     <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="7" width="8.7265625" customWidth="1"/>
     <col min="8" max="8" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.7265625" customWidth="1"/>
     <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" customWidth="1"/>
     <col min="16" max="16" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7265625" customWidth="1"/>
     <col min="23" max="23" width="20.08984375" customWidth="1"/>
     <col min="24" max="24" width="14.7265625" customWidth="1"/>
     <col min="25" max="25" width="23.7265625" customWidth="1"/>
@@ -1667,143 +1786,146 @@
     <col min="27" max="27" width="19.1796875" customWidth="1"/>
     <col min="28" max="28" width="14.08984375" customWidth="1"/>
     <col min="29" max="29" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="44" width="8.7265625" customWidth="1"/>
     <col min="45" max="45" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="8.7265625" customWidth="1"/>
+    <col min="49" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:45" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="12" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1815,7 +1937,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -1906,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -1993,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2070,7 +2192,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2147,7 +2269,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -2230,7 +2352,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
@@ -2313,7 +2435,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Fixed many test cases under nitrox buy sell feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3BAB8C-4757-4E88-99A3-5EF5BAE888C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE272DD-4B10-46E5-8FF4-0898D0BABFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -950,9 +950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I25" sqref="I25"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modified Bots and added new Test case37
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE272DD-4B10-46E5-8FF4-0898D0BABFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA3E38F-90D2-4388-B5FD-C95B67C96949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -950,9 +950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1718,7 +1718,7 @@
         <v>103</v>
       </c>
       <c r="I22" s="8">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
added the test case38
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA3E38F-90D2-4388-B5FD-C95B67C96949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C4CA2D-E9F2-4BD5-8A2E-D48C7B371341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -368,6 +368,18 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_037</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_038</t>
+  </si>
+  <si>
+    <t>Mside</t>
+  </si>
+  <si>
+    <t>LONG</t>
+  </si>
+  <si>
+    <t>LTC/USDT Perpetual USDT</t>
   </si>
 </sst>
 </file>
@@ -377,7 +389,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +418,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -463,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -489,6 +507,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -950,9 +969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,28 +981,28 @@
     <col min="3" max="3" width="28.81640625" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.7265625" customWidth="1"/>
     <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.7265625" customWidth="1"/>
-    <col min="17" max="17" width="34.1796875" customWidth="1"/>
-    <col min="18" max="18" width="8.7265625" customWidth="1"/>
-    <col min="19" max="19" width="8.08984375" customWidth="1"/>
-    <col min="20" max="26" width="8.7265625" customWidth="1"/>
-    <col min="27" max="16379" width="8.7265625" hidden="1"/>
-    <col min="16380" max="16380" width="25.26953125" hidden="1"/>
-    <col min="16381" max="16381" width="16.90625" hidden="1"/>
-    <col min="16382" max="16382" width="26.6328125" hidden="1"/>
-    <col min="16383" max="16383" width="15.453125" hidden="1"/>
-    <col min="16384" max="16384" width="2.90625" hidden="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.7265625" customWidth="1"/>
+    <col min="18" max="18" width="34.1796875" customWidth="1"/>
+    <col min="19" max="19" width="8.7265625" customWidth="1"/>
+    <col min="20" max="20" width="8.08984375" customWidth="1"/>
+    <col min="21" max="27" width="8.7265625" customWidth="1"/>
+    <col min="28" max="16380" width="8.7265625" hidden="1"/>
+    <col min="16381" max="16381" width="25.26953125" hidden="1"/>
+    <col min="16382" max="16382" width="16.90625" hidden="1"/>
+    <col min="16383" max="16383" width="26.6328125" hidden="1"/>
+    <col min="16384" max="16384" width="15.453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1018,31 +1037,34 @@
         <v>11</v>
       </c>
       <c r="L1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1054,6 +1076,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1066,11 +1089,12 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1080,6 +1104,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1092,11 +1117,12 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1106,6 +1132,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1118,11 +1145,12 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1132,6 +1160,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1144,11 +1173,12 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1160,6 +1190,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1172,11 +1203,12 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1186,6 +1218,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1198,11 +1231,12 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S7" s="2"/>
+      <c r="T7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1214,6 +1248,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1226,11 +1261,12 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1246,6 +1282,7 @@
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1258,11 +1295,12 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S9" s="2"/>
+      <c r="T9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1278,6 +1316,7 @@
       <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1290,11 +1329,12 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1310,6 +1350,7 @@
       <c r="E11" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1319,18 +1360,19 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1346,6 +1388,7 @@
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1353,20 +1396,21 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1382,6 +1426,7 @@
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1391,18 +1436,19 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S13" s="2"/>
+      <c r="T13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1418,6 +1464,7 @@
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1427,18 +1474,19 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1454,6 +1502,7 @@
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1463,18 +1512,19 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2">
+        <v>1</v>
+      </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S15" s="2"/>
+      <c r="T15" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1490,6 +1540,7 @@
       <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1504,11 +1555,12 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S16" s="2"/>
+      <c r="T16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
@@ -1534,22 +1586,23 @@
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7">
-        <v>1</v>
-      </c>
-      <c r="O17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7">
+        <v>1</v>
+      </c>
       <c r="P17" s="7"/>
-      <c r="Q17" s="7">
-        <v>1</v>
-      </c>
+      <c r="Q17" s="7"/>
       <c r="R17" s="7">
         <v>1</v>
       </c>
-      <c r="S17" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S17" s="7">
+        <v>1</v>
+      </c>
+      <c r="T17" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>102</v>
       </c>
@@ -1574,20 +1627,27 @@
       <c r="K18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2">
+      <c r="O18" s="2">
         <v>1</v>
       </c>
       <c r="R18" s="2">
         <v>1</v>
       </c>
-      <c r="S18" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S18" s="2">
+        <v>1</v>
+      </c>
+      <c r="T18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+    </row>
+    <row r="19" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>107</v>
       </c>
@@ -1612,20 +1672,27 @@
       <c r="K19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N19" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="2">
+      <c r="O19" s="2">
         <v>1</v>
       </c>
       <c r="R19" s="2">
         <v>1</v>
       </c>
-      <c r="S19" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S19" s="2">
+        <v>1</v>
+      </c>
+      <c r="T19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+    </row>
+    <row r="20" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>112</v>
       </c>
@@ -1636,7 +1703,7 @@
         <v>101</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>103</v>
@@ -1650,20 +1717,30 @@
       <c r="K20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2">
+      <c r="L20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O20" s="2">
         <v>1</v>
       </c>
       <c r="R20" s="2">
         <v>1</v>
       </c>
-      <c r="S20" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S20" s="2">
+        <v>1</v>
+      </c>
+      <c r="T20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+    </row>
+    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>115</v>
       </c>
@@ -1674,7 +1751,7 @@
         <v>101</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>103</v>
@@ -1688,20 +1765,30 @@
       <c r="K21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N21" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="2">
+      <c r="L21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O21" s="2">
         <v>1</v>
       </c>
       <c r="R21" s="2">
         <v>1</v>
       </c>
-      <c r="S21" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="S21" s="2">
+        <v>1</v>
+      </c>
+      <c r="T21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+    </row>
+    <row r="22" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>116</v>
       </c>
@@ -1726,18 +1813,71 @@
       <c r="K22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="2">
+      <c r="L22" s="13"/>
+      <c r="O22" s="2">
         <v>1</v>
       </c>
       <c r="R22" s="2">
         <v>1</v>
       </c>
-      <c r="S22" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+    </row>
+    <row r="23" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="8">
+        <v>25</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>

</xml_diff>

<commit_message>
Autmated QA_TestCase_Auto_NitroX_039 and modified buysell testcase18
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C4CA2D-E9F2-4BD5-8A2E-D48C7B371341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A766D5-D50F-4D13-98E5-1393B6A9862A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="122">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -379,7 +379,10 @@
     <t>LONG</t>
   </si>
   <si>
-    <t>LTC/USDT Perpetual USDT</t>
+    <t>QA_TestCase_Auto_NitroX_039</t>
+  </si>
+  <si>
+    <t>XRP/USDT Perpetual USDT</t>
   </si>
 </sst>
 </file>
@@ -969,9 +972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1085,7 +1088,9 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1113,7 +1118,9 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1141,7 +1148,9 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -1169,7 +1178,9 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1199,7 +1210,9 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -1227,7 +1240,9 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -1257,7 +1272,9 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1291,7 +1308,9 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1325,7 +1344,9 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1551,7 +1572,9 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1703,7 +1726,7 @@
         <v>101</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>103</v>
@@ -1721,7 +1744,7 @@
         <v>119</v>
       </c>
       <c r="O20" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R20" s="2">
         <v>1</v>
@@ -1751,7 +1774,7 @@
         <v>101</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>103</v>
@@ -1769,7 +1792,7 @@
         <v>119</v>
       </c>
       <c r="O21" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R21" s="2">
         <v>1</v>
@@ -1799,7 +1822,7 @@
         <v>101</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>103</v>
@@ -1815,7 +1838,7 @@
       </c>
       <c r="L22" s="13"/>
       <c r="O22" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="R22" s="2">
         <v>1</v>
@@ -1878,6 +1901,51 @@
       <c r="Y23"/>
       <c r="Z23"/>
       <c r="AA23"/>
+    </row>
+    <row r="24" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="8">
+        <v>25</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1</v>
+      </c>
+      <c r="T24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1"/>

</xml_diff>

<commit_message>
Implemented env name as a maven argument
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1601F64A-8578-41C5-B8E8-AA74F037B044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A70091-6550-4C35-80D8-C3FFDA296767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="129">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -277,9 +277,6 @@
     <t>SPOT</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_040</t>
-  </si>
-  <si>
-    <t>https://staging-nitrox.altono.app</t>
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_041</t>
@@ -419,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,14 +424,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -507,11 +493,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -526,13 +511,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -871,25 +854,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878D5118-86AA-443A-B8A4-36B93CD796C0}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.7265625" customWidth="1"/>
-    <col min="2" max="2" width="48.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="66.1796875" customWidth="1"/>
-    <col min="8" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="66.1796875" customWidth="1"/>
+    <col min="7" max="25" width="8.7265625" customWidth="1"/>
     <col min="27" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -903,91 +885,76 @@
         <v>88</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://system.qa/" xr:uid="{ADDE2EEE-F6B9-40ED-AA61-6A610598917E}"/>
-    <hyperlink ref="C4" r:id="rId2" display="http://system.qa/" xr:uid="{94FF34FB-97BA-43C4-9AF6-736D81B5AAA4}"/>
-    <hyperlink ref="B2" r:id="rId3" display="https://staging-nitrox.altono.app/" xr:uid="{5BB33F06-A9FD-4B13-8234-AA3309C42662}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://staging-nitrox.altono.app/" xr:uid="{826BA71D-F9AC-43A2-BF34-2F92209214A7}"/>
-    <hyperlink ref="B4" r:id="rId5" display="https://staging-nitrox.altono.app/" xr:uid="{6950D2D8-FD65-4EAD-9B9E-0ED7C491D8BB}"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://system.qa/" xr:uid="{ADDE2EEE-F6B9-40ED-AA61-6A610598917E}"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://system.qa/" xr:uid="{94FF34FB-97BA-43C4-9AF6-736D81B5AAA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1044,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>9</v>
@@ -1053,19 +1020,19 @@
         <v>10</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>12</v>
@@ -1257,7 +1224,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1290,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1323,7 +1290,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -1360,7 +1327,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -1397,7 +1364,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
@@ -1436,7 +1403,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>29</v>
@@ -1475,7 +1442,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
@@ -1514,7 +1481,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -1553,7 +1520,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -1592,7 +1559,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -1631,7 +1598,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>29</v>
@@ -1668,25 +1635,25 @@
     </row>
     <row r="18" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" s="6">
         <v>25</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>32</v>
@@ -1713,25 +1680,25 @@
     </row>
     <row r="19" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I19" s="6">
         <v>25</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>32</v>
@@ -1758,31 +1725,31 @@
     </row>
     <row r="20" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="6">
         <v>25</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P20" s="2">
         <v>20</v>
@@ -1806,31 +1773,31 @@
     </row>
     <row r="21" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" s="6">
         <v>25</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P21" s="2">
         <v>20</v>
@@ -1854,30 +1821,30 @@
     </row>
     <row r="22" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I22" s="6">
         <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="11"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="9"/>
       <c r="P22" s="2">
         <v>20</v>
@@ -1901,25 +1868,25 @@
     </row>
     <row r="23" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I23" s="6">
         <v>25</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>37</v>
@@ -1946,25 +1913,25 @@
     </row>
     <row r="24" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I24" s="6">
         <v>25</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>37</v>
@@ -1991,25 +1958,25 @@
     </row>
     <row r="25" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25" s="6">
         <v>25</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>37</v>
@@ -2036,25 +2003,25 @@
     </row>
     <row r="26" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I26" s="6">
         <v>25</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>37</v>
@@ -2106,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AM1" sqref="AM1"/>
     </sheetView>
@@ -2165,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>9</v>
@@ -2174,10 +2141,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>40</v>
@@ -2189,10 +2156,10 @@
         <v>42</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>62</v>
@@ -2219,10 +2186,10 @@
         <v>49</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Z1" s="8" t="s">
         <v>50</v>
@@ -2264,7 +2231,7 @@
         <v>62</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AN1" s="8" t="s">
         <v>11</v>
@@ -2314,7 +2281,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2412,7 +2379,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2506,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2590,7 +2557,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -2674,7 +2641,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -2690,13 +2657,13 @@
         <v>71</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>32</v>
@@ -2763,7 +2730,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
@@ -2780,13 +2747,13 @@
         <v>71</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M7" s="2">
         <v>1</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>77</v>
@@ -2853,7 +2820,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
@@ -2939,28 +2906,28 @@
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I9" s="6">
         <v>25</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>71</v>
@@ -2994,7 +2961,7 @@
         <v>73</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Y9" s="2">
         <v>3000</v>
@@ -3045,28 +3012,28 @@
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I10" s="6">
         <v>25</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>71</v>
@@ -3100,7 +3067,7 @@
         <v>73</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Y10" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Modified the existing Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4BB598-C388-4A6D-B3FB-CC2CE2EEA095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5963C8A5-8892-45B0-8B7A-B57D8036D406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="155">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_021</t>
+  </si>
+  <si>
+    <t>QA_TestCase_Auto_NitroX_022</t>
   </si>
 </sst>
 </file>
@@ -2179,11 +2182,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
-  <dimension ref="A1:BG32"/>
+  <dimension ref="A1:BG33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2610,7 +2613,7 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
@@ -2714,7 +2717,7 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
@@ -2744,12 +2747,12 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="S5" s="2">
         <v>20</v>
@@ -2757,7 +2760,9 @@
       <c r="T5" s="2">
         <v>50</v>
       </c>
-      <c r="U5" s="2"/>
+      <c r="U5" s="2">
+        <v>0.2</v>
+      </c>
       <c r="V5" s="2"/>
       <c r="W5" s="7">
         <v>0.1</v>
@@ -2770,10 +2775,10 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2">
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="AD5" s="2">
-        <v>3900</v>
+        <v>4000</v>
       </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
@@ -2787,7 +2792,9 @@
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
+      <c r="AO5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="AP5" s="2"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
@@ -2808,11 +2815,13 @@
         <v>0</v>
       </c>
       <c r="BC5" s="2"/>
-      <c r="BD5" s="2"/>
+      <c r="BD5" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>85</v>
@@ -2835,55 +2844,65 @@
         <v>71</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="R6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="2">
+        <v>20</v>
+      </c>
+      <c r="T6" s="2">
+        <v>50</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="W6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
+      <c r="AC6" s="2">
+        <v>3100</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>3900</v>
+      </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
+      <c r="AK6" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AO6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP6" s="2">
-        <v>1</v>
-      </c>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
-      <c r="AR6" s="2">
-        <v>3000</v>
-      </c>
-      <c r="AS6" s="2">
-        <v>4000</v>
-      </c>
-      <c r="AT6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2">
+        <v>1</v>
+      </c>
       <c r="AV6" s="2"/>
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
@@ -2900,7 +2919,7 @@
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>85</v>
@@ -2956,7 +2975,7 @@
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="AP7" s="2">
         <v>1</v>
@@ -2988,7 +3007,7 @@
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>85</v>
@@ -3002,6 +3021,7 @@
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="6"/>
@@ -3010,17 +3030,13 @@
         <v>71</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="M8" s="2">
         <v>1</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -3047,10 +3063,10 @@
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="AP8" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2">
@@ -3062,12 +3078,8 @@
       <c r="AT8" s="2">
         <v>1</v>
       </c>
-      <c r="AU8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="2">
-        <v>2</v>
-      </c>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
@@ -3083,7 +3095,7 @@
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>85</v>
@@ -3097,7 +3109,6 @@
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="6"/>
@@ -3115,7 +3126,7 @@
         <v>108</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -3143,7 +3154,7 @@
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="AP9" s="2">
         <v>0.1</v>
@@ -3161,7 +3172,9 @@
       <c r="AU9" s="2">
         <v>1</v>
       </c>
-      <c r="AV9" s="2"/>
+      <c r="AV9" s="2">
+        <v>2</v>
+      </c>
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
@@ -3177,13 +3190,13 @@
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -3200,13 +3213,17 @@
         <v>71</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="M10" s="2">
         <v>1</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -3231,11 +3248,9 @@
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
-      <c r="AN10" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="AN10" s="2"/>
       <c r="AO10" s="2" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="AP10" s="2">
         <v>0.1</v>
@@ -3251,16 +3266,12 @@
         <v>1</v>
       </c>
       <c r="AU10" s="2">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="AV10" s="2"/>
-      <c r="AW10" s="11">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AX10" s="11"/>
-      <c r="AY10" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
       <c r="AZ10" s="2">
         <v>1</v>
       </c>
@@ -3273,7 +3284,7 @@
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>85</v>
@@ -3331,7 +3342,7 @@
         <v>32</v>
       </c>
       <c r="AO11" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="AP11" s="2">
         <v>0.1</v>
@@ -3369,7 +3380,7 @@
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>85</v>
@@ -3424,10 +3435,10 @@
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO12" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="AO12" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AP12" s="2">
         <v>0.1</v>
@@ -3465,7 +3476,7 @@
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>85</v>
@@ -3520,10 +3531,10 @@
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="AO13" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="AP13" s="2">
         <v>0.1</v>
@@ -3542,10 +3553,10 @@
         <v>0.01</v>
       </c>
       <c r="AV13" s="2"/>
-      <c r="AW13" s="12">
+      <c r="AW13" s="11">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX13" s="12"/>
+      <c r="AX13" s="11"/>
       <c r="AY13" s="2" t="s">
         <v>85</v>
       </c>
@@ -3561,102 +3572,90 @@
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" s="6">
-        <v>25</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="M14" s="2">
         <v>1</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S14" s="2">
-        <v>20</v>
-      </c>
-      <c r="T14" s="2">
-        <v>50</v>
-      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="7">
-        <v>20</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>1200</v>
-      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AD14" s="2">
-        <v>0.5</v>
-      </c>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
-      <c r="AK14" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
+      <c r="AN14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="AO14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP14" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>0.1</v>
+      </c>
       <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
+      <c r="AR14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AT14" s="2">
+        <v>1</v>
+      </c>
       <c r="AU14" s="2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="AV14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AX14" s="2"/>
-      <c r="AY14" s="2"/>
+      <c r="AW14" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="AZ14" s="2">
         <v>1</v>
       </c>
@@ -3665,13 +3664,11 @@
         <v>0</v>
       </c>
       <c r="BC14" s="2"/>
-      <c r="BD14" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="BD14" s="2"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -3710,7 +3707,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="S15" s="2">
         <v>20</v>
@@ -3721,7 +3718,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="7">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>73</v>
@@ -3730,7 +3727,7 @@
         <v>124</v>
       </c>
       <c r="Z15" s="2">
-        <v>1</v>
+        <v>1200</v>
       </c>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
@@ -3781,7 +3778,7 @@
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -3789,69 +3786,89 @@
       <c r="C16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
         <v>119</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="6">
+        <v>25</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="K16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M16" s="2">
         <v>1</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
+      <c r="R16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="S16" s="2">
+        <v>20</v>
+      </c>
+      <c r="T16" s="2">
+        <v>50</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
+      <c r="W16" s="7">
+        <v>50</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1</v>
+      </c>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
+      <c r="AC16" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>0.5</v>
+      </c>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
+      <c r="AK16" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AP16" s="2">
-        <v>20</v>
-      </c>
+      <c r="AP16" s="2"/>
       <c r="AQ16" s="2"/>
-      <c r="AR16" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AS16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AT16" s="2">
-        <v>1</v>
-      </c>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
       <c r="AU16" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="AV16" s="2"/>
       <c r="AW16" s="2"/>
@@ -3865,11 +3882,13 @@
         <v>0</v>
       </c>
       <c r="BC16" s="2"/>
-      <c r="BD16" s="2"/>
+      <c r="BD16" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -3923,7 +3942,7 @@
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="AP17" s="2">
         <v>20</v>
@@ -3957,89 +3976,77 @@
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
         <v>71</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="M18" s="2">
         <v>1</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S18" s="2">
-        <v>20</v>
-      </c>
-      <c r="T18" s="2">
-        <v>50</v>
-      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
-      <c r="AC18" s="2">
-        <v>3000</v>
-      </c>
-      <c r="AD18" s="2">
-        <v>4000</v>
-      </c>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
-      <c r="AK18" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP18" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="AP18" s="2">
+        <v>20</v>
+      </c>
       <c r="AQ18" s="2"/>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AT18" s="2"/>
+      <c r="AR18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AS18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AT18" s="2">
+        <v>1</v>
+      </c>
       <c r="AU18" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
@@ -4053,13 +4060,11 @@
         <v>0</v>
       </c>
       <c r="BC18" s="2"/>
-      <c r="BD18" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="BD18" s="2"/>
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>85</v>
@@ -4161,7 +4166,7 @@
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>85</v>
@@ -4263,7 +4268,7 @@
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>85</v>
@@ -4365,7 +4370,7 @@
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>85</v>
@@ -4467,7 +4472,7 @@
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>85</v>
@@ -4510,9 +4515,7 @@
       <c r="T23" s="2">
         <v>50</v>
       </c>
-      <c r="U23" s="2">
-        <v>0.2</v>
-      </c>
+      <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="7">
         <v>0.1</v>
@@ -4571,7 +4574,7 @@
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>85</v>
@@ -4594,57 +4597,69 @@
         <v>71</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M24" s="2">
         <v>1</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="O24" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
+      <c r="R24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24" s="2">
+        <v>20</v>
+      </c>
+      <c r="T24" s="2">
+        <v>50</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.2</v>
+      </c>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
+      <c r="W24" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
+      <c r="AC24" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
-      <c r="AK24" s="2"/>
+      <c r="AK24" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AP24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ24" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR24" s="2">
-        <v>3000</v>
-      </c>
-      <c r="AS24" s="2">
-        <v>4000</v>
-      </c>
-      <c r="AT24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2">
+        <v>1</v>
+      </c>
       <c r="AV24" s="2"/>
       <c r="AW24" s="2"/>
       <c r="AX24" s="2"/>
@@ -4657,17 +4672,19 @@
         <v>0</v>
       </c>
       <c r="BC24" s="2"/>
-      <c r="BD24" s="2"/>
+      <c r="BD24" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -4684,7 +4701,7 @@
         <v>71</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="M25" s="2">
         <v>1</v>
@@ -4715,16 +4732,16 @@
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
-      <c r="AN25" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="AN25" s="2"/>
       <c r="AO25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="AP25" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AQ25" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="2">
+        <v>2</v>
+      </c>
       <c r="AR25" s="2">
         <v>3000</v>
       </c>
@@ -4734,19 +4751,11 @@
       <c r="AT25" s="2">
         <v>1</v>
       </c>
-      <c r="AU25" s="2">
-        <v>0.01</v>
-      </c>
+      <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
-      <c r="AW25" s="11">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AX25" s="11">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AY25" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
       <c r="AZ25" s="2">
         <v>1</v>
       </c>
@@ -4759,13 +4768,13 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>29</v>
@@ -4782,73 +4791,69 @@
         <v>71</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="M26" s="2">
         <v>1</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S26" s="2">
-        <v>20</v>
-      </c>
-      <c r="T26" s="2">
-        <v>50</v>
-      </c>
-      <c r="U26" s="2">
-        <v>0.2</v>
-      </c>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="X26" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
-      <c r="AC26" s="2">
-        <v>3000</v>
-      </c>
-      <c r="AD26" s="2">
-        <v>4000</v>
-      </c>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="2"/>
-      <c r="AK26" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
-      <c r="AN26" s="2"/>
+      <c r="AN26" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="AO26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AP26" s="2"/>
+      <c r="AP26" s="2">
+        <v>0.1</v>
+      </c>
       <c r="AQ26" s="2"/>
-      <c r="AR26" s="2"/>
-      <c r="AS26" s="2"/>
-      <c r="AT26" s="2"/>
+      <c r="AR26" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AS26" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AT26" s="2">
+        <v>1</v>
+      </c>
       <c r="AU26" s="2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="AV26" s="2"/>
-      <c r="AW26" s="2"/>
-      <c r="AX26" s="2"/>
-      <c r="AY26" s="2"/>
+      <c r="AW26" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AX26" s="11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AY26" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="AZ26" s="2">
         <v>1</v>
       </c>
@@ -4857,13 +4862,11 @@
         <v>0</v>
       </c>
       <c r="BC26" s="2"/>
-      <c r="BD26" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="BD26" s="2"/>
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>85</v>
@@ -4886,57 +4889,69 @@
         <v>71</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M27" s="2">
         <v>1</v>
       </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
+      <c r="O27" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
+      <c r="R27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S27" s="2">
+        <v>20</v>
+      </c>
+      <c r="T27" s="2">
+        <v>50</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0.2</v>
+      </c>
       <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
+      <c r="W27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
-      <c r="AC27" s="2"/>
-      <c r="AD27" s="2"/>
+      <c r="AC27" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="2"/>
-      <c r="AK27" s="2"/>
+      <c r="AK27" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AL27" s="2"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AP27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ27" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR27" s="2">
-        <v>3000</v>
-      </c>
-      <c r="AS27" s="2">
-        <v>4000</v>
-      </c>
-      <c r="AT27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2">
+        <v>1</v>
+      </c>
       <c r="AV27" s="2"/>
       <c r="AW27" s="2"/>
       <c r="AX27" s="2"/>
@@ -4949,17 +4964,19 @@
         <v>0</v>
       </c>
       <c r="BC27" s="2"/>
-      <c r="BD27" s="2"/>
+      <c r="BD27" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>29</v>
@@ -4976,7 +4993,7 @@
         <v>71</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="M28" s="2">
         <v>1</v>
@@ -5007,16 +5024,16 @@
       <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
       <c r="AM28" s="2"/>
-      <c r="AN28" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="AN28" s="2"/>
       <c r="AO28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="AP28" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="AQ28" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="AQ28" s="2">
+        <v>2</v>
+      </c>
       <c r="AR28" s="2">
         <v>3000</v>
       </c>
@@ -5026,19 +5043,11 @@
       <c r="AT28" s="2">
         <v>1</v>
       </c>
-      <c r="AU28" s="2">
-        <v>0.01</v>
-      </c>
+      <c r="AU28" s="2"/>
       <c r="AV28" s="2"/>
-      <c r="AW28" s="11">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="AX28" s="11">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AY28" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
       <c r="AZ28" s="2">
         <v>1</v>
       </c>
@@ -5051,13 +5060,13 @@
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>29</v>
@@ -5065,6 +5074,7 @@
       <c r="E29" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="6"/>
@@ -5073,17 +5083,13 @@
         <v>71</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="M29" s="2">
         <v>1</v>
       </c>
-      <c r="N29" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -5108,7 +5114,9 @@
       <c r="AK29" s="2"/>
       <c r="AL29" s="2"/>
       <c r="AM29" s="2"/>
-      <c r="AN29" s="2"/>
+      <c r="AN29" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="AO29" s="2" t="s">
         <v>32</v>
       </c>
@@ -5126,14 +5134,18 @@
         <v>1</v>
       </c>
       <c r="AU29" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV29" s="2">
-        <v>2</v>
-      </c>
-      <c r="AW29" s="2"/>
-      <c r="AX29" s="2"/>
-      <c r="AY29" s="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AX29" s="11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AY29" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="AZ29" s="2">
         <v>1</v>
       </c>
@@ -5144,11 +5156,106 @@
       <c r="BC29" s="2"/>
       <c r="BD29" s="2"/>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="F32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="2"/>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP30" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AS30" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AT30" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU30" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV30" s="2">
+        <v>2</v>
+      </c>
+      <c r="AW30" s="2"/>
+      <c r="AX30" s="2"/>
+      <c r="AY30" s="2"/>
+      <c r="AZ30" s="2">
+        <v>1</v>
+      </c>
+      <c r="BA30" s="2"/>
+      <c r="BB30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="2"/>
+      <c r="BD30" s="2"/>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified Script for Bots
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737FC5F9-F8C6-4271-A56D-B468E714E5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEBE586-0E87-471B-8253-23E9C368A3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="207">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -517,9 +517,6 @@
     <t>QA_TestCase_Auto_NitroX_096</t>
   </si>
   <si>
-    <t>test@Binancedm</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_050</t>
   </si>
   <si>
@@ -574,9 +571,6 @@
     <t>QA_TestCase_Auto_NitroX_054</t>
   </si>
   <si>
-    <t>test@Ftx.</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_055</t>
   </si>
   <si>
@@ -638,6 +632,12 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_106</t>
+  </si>
+  <si>
+    <t>ETH/USD Perpetual USD</t>
+  </si>
+  <si>
+    <t>test@Ftx</t>
   </si>
 </sst>
 </file>
@@ -2346,9 +2346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BG80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AS87" sqref="AS87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3558,15 +3558,17 @@
         <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="6"/>
@@ -3654,15 +3656,17 @@
         <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="6"/>
@@ -3750,15 +3754,17 @@
         <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
@@ -3846,15 +3852,17 @@
         <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="6"/>
@@ -3936,18 +3944,18 @@
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -4040,18 +4048,18 @@
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4144,18 +4152,18 @@
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4248,18 +4256,18 @@
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -4358,12 +4366,12 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
@@ -4468,12 +4476,12 @@
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -4578,12 +4586,12 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -4668,10 +4676,13 @@
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -4749,13 +4760,13 @@
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
@@ -4764,7 +4775,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -4849,13 +4860,13 @@
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -4864,7 +4875,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -4949,13 +4960,13 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>29</v>
@@ -4964,7 +4975,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -5047,13 +5058,13 @@
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
@@ -5062,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -5145,13 +5156,13 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>29</v>
@@ -5160,7 +5171,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -5243,13 +5254,13 @@
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>29</v>
@@ -5258,7 +5269,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -6565,7 +6576,7 @@
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>85</v>
@@ -7060,13 +7071,13 @@
     </row>
     <row r="47" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>29</v>
@@ -7075,7 +7086,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -7166,13 +7177,13 @@
     </row>
     <row r="48" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>29</v>
@@ -7181,7 +7192,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -7272,13 +7283,13 @@
     </row>
     <row r="49" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>29</v>
@@ -7287,7 +7298,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -7378,13 +7389,13 @@
     </row>
     <row r="50" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>29</v>
@@ -7393,7 +7404,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -7484,13 +7495,13 @@
     </row>
     <row r="51" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>29</v>
@@ -7499,7 +7510,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -7590,13 +7601,13 @@
     </row>
     <row r="52" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>29</v>
@@ -7605,7 +7616,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -7698,13 +7709,13 @@
     </row>
     <row r="53" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>29</v>
@@ -7713,7 +7724,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -7804,13 +7815,13 @@
     </row>
     <row r="54" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>29</v>
@@ -7819,7 +7830,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -7912,13 +7923,13 @@
     </row>
     <row r="55" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>29</v>
@@ -7927,7 +7938,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -8020,13 +8031,13 @@
     </row>
     <row r="56" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>29</v>
@@ -8035,7 +8046,7 @@
         <v>2</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -8089,10 +8100,10 @@
         <v>2</v>
       </c>
       <c r="AR56" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="AS56" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="AT56" s="2">
         <v>1</v>
@@ -8116,13 +8127,13 @@
     </row>
     <row r="57" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
@@ -8131,7 +8142,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -8185,10 +8196,10 @@
         <v>2</v>
       </c>
       <c r="AR57" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="AS57" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="AT57" s="2">
         <v>1</v>
@@ -8212,13 +8223,13 @@
     </row>
     <row r="58" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>29</v>
@@ -8227,7 +8238,7 @@
         <v>2</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -8314,13 +8325,13 @@
     </row>
     <row r="59" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>29</v>
@@ -8329,7 +8340,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -8416,13 +8427,13 @@
     </row>
     <row r="60" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>29</v>
@@ -8431,7 +8442,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -8524,13 +8535,13 @@
     </row>
     <row r="61" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>29</v>
@@ -8539,7 +8550,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -8618,13 +8629,13 @@
     </row>
     <row r="62" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>29</v>
@@ -8633,7 +8644,7 @@
         <v>2</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -8720,13 +8731,13 @@
     </row>
     <row r="63" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>29</v>
@@ -8735,7 +8746,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -9548,13 +9559,13 @@
     </row>
     <row r="71" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>29</v>
@@ -9563,7 +9574,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -9656,13 +9667,13 @@
     </row>
     <row r="72" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>29</v>
@@ -9671,7 +9682,7 @@
         <v>2</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -9718,10 +9729,10 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
       <c r="AC72" s="2">
-        <v>1200</v>
+        <v>3000</v>
       </c>
       <c r="AD72" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="AE72" s="2"/>
       <c r="AF72" s="2"/>
@@ -9764,13 +9775,13 @@
     </row>
     <row r="73" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>29</v>
@@ -9779,7 +9790,7 @@
         <v>2</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -9811,8 +9822,12 @@
       </c>
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
-      <c r="AC73" s="2"/>
-      <c r="AD73" s="2"/>
+      <c r="AC73" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD73" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE73" s="2"/>
       <c r="AF73" s="2"/>
       <c r="AG73" s="2"/>
@@ -9833,10 +9848,10 @@
         <v>2</v>
       </c>
       <c r="AR73" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="AS73" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="AT73" s="2">
         <v>1</v>
@@ -9860,13 +9875,13 @@
     </row>
     <row r="74" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>29</v>
@@ -9875,7 +9890,7 @@
         <v>2</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -9907,8 +9922,12 @@
       </c>
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
-      <c r="AC74" s="2"/>
-      <c r="AD74" s="2"/>
+      <c r="AC74" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD74" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE74" s="2"/>
       <c r="AF74" s="2"/>
       <c r="AG74" s="2"/>
@@ -9929,10 +9948,10 @@
         <v>2</v>
       </c>
       <c r="AR74" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="AS74" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="AT74" s="2">
         <v>1</v>
@@ -9956,13 +9975,13 @@
     </row>
     <row r="75" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>29</v>
@@ -9971,7 +9990,7 @@
         <v>2</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -10003,8 +10022,12 @@
       </c>
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
-      <c r="AC75" s="2"/>
-      <c r="AD75" s="2"/>
+      <c r="AC75" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD75" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE75" s="2"/>
       <c r="AF75" s="2"/>
       <c r="AG75" s="2"/>
@@ -10058,13 +10081,13 @@
     </row>
     <row r="76" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>29</v>
@@ -10073,7 +10096,7 @@
         <v>2</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -10105,8 +10128,12 @@
       </c>
       <c r="AA76" s="2"/>
       <c r="AB76" s="2"/>
-      <c r="AC76" s="2"/>
-      <c r="AD76" s="2"/>
+      <c r="AC76" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AD76" s="2">
+        <v>4000</v>
+      </c>
       <c r="AE76" s="2"/>
       <c r="AF76" s="2"/>
       <c r="AG76" s="2"/>
@@ -10160,13 +10187,13 @@
     </row>
     <row r="77" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>29</v>
@@ -10175,7 +10202,7 @@
         <v>2</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -10268,13 +10295,13 @@
     </row>
     <row r="78" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>29</v>
@@ -10283,7 +10310,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -10362,13 +10389,13 @@
     </row>
     <row r="79" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>29</v>
@@ -10377,7 +10404,7 @@
         <v>2</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -10464,13 +10491,13 @@
     </row>
     <row r="80" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>29</v>
@@ -10479,7 +10506,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>

</xml_diff>

<commit_message>
Updated the Excel Sheet with ftx Account
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEBE586-0E87-471B-8253-23E9C368A3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD971C81-1B10-475C-9450-1E2B098CB461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2346,9 +2346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BG80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS87" sqref="AS87"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Locators ,NitroX Update
Updated the NitroX test cases.Added locators for Optimus and Optimzed XAlpha
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE877E-2F14-4C21-B4AA-8C3E69D2466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B25CC-2A33-4B36-9BE1-8761C6E2EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -1258,9 +1258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B19" sqref="B19"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1642,7 +1642,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -2397,7 +2397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BG97" sqref="BG97"/>
     </sheetView>

</xml_diff>

<commit_message>
Optimized the changes in Nitrox
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B25CC-2A33-4B36-9BE1-8761C6E2EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCADEE-6FEE-4849-A232-81686821DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="222">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -313,12 +313,6 @@
     <t>Instrument</t>
   </si>
   <si>
-    <t>ETH/USDT Perpetual USDT</t>
-  </si>
-  <si>
-    <t>QUANT_BINANCEDM_25</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_034</t>
   </si>
   <si>
@@ -376,9 +370,6 @@
     <t>QA_TestCase_Auto_NitroX_039</t>
   </si>
   <si>
-    <t>XRP/USDT Perpetual USDT</t>
-  </si>
-  <si>
     <t>QA_TestCase_Auto_NitroX_040</t>
   </si>
   <si>
@@ -689,6 +680,9 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_123</t>
+  </si>
+  <si>
+    <t>XRP/USD Perpetual USD</t>
   </si>
 </sst>
 </file>
@@ -1258,9 +1252,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1316,19 +1310,19 @@
         <v>10</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>12</v>
@@ -1520,7 +1514,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1553,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1586,7 +1580,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -1623,7 +1617,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -1660,7 +1654,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
@@ -1699,7 +1693,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>29</v>
@@ -1738,7 +1732,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
@@ -1777,7 +1771,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -1816,7 +1810,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -1855,7 +1849,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -1894,7 +1888,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>29</v>
@@ -1931,25 +1925,25 @@
     </row>
     <row r="18" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I18" s="6">
         <v>25</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>32</v>
@@ -1976,25 +1970,25 @@
     </row>
     <row r="19" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I19" s="6">
         <v>25</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>32</v>
@@ -2021,34 +2015,34 @@
     </row>
     <row r="20" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I20" s="6">
         <v>25</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P20" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S20" s="2">
         <v>1</v>
@@ -2069,34 +2063,34 @@
     </row>
     <row r="21" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I21" s="6">
         <v>25</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P21" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S21" s="2">
         <v>1</v>
@@ -2117,25 +2111,25 @@
     </row>
     <row r="22" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I22" s="6">
         <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>32</v>
@@ -2143,7 +2137,7 @@
       <c r="L22" s="10"/>
       <c r="M22" s="9"/>
       <c r="P22" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S22" s="2">
         <v>1</v>
@@ -2164,25 +2158,25 @@
     </row>
     <row r="23" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I23" s="6">
         <v>25</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>37</v>
@@ -2209,25 +2203,25 @@
     </row>
     <row r="24" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I24" s="6">
         <v>25</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>37</v>
@@ -2254,31 +2248,31 @@
     </row>
     <row r="25" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I25" s="6">
         <v>25</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="P25" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S25" s="2">
         <v>1</v>
@@ -2299,31 +2293,31 @@
     </row>
     <row r="26" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="I26" s="6">
         <v>25</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="P26" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="S26" s="2">
         <v>1</v>
@@ -2344,13 +2338,13 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
@@ -2397,9 +2391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BG97"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BG97" sqref="BG97"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2472,10 +2466,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>40</v>
@@ -2487,10 +2481,10 @@
         <v>42</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>62</v>
@@ -2508,7 +2502,7 @@
         <v>46</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="V1" s="8" t="s">
         <v>47</v>
@@ -2520,10 +2514,10 @@
         <v>49</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AA1" s="8" t="s">
         <v>50</v>
@@ -2565,7 +2559,7 @@
         <v>62</v>
       </c>
       <c r="AN1" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AO1" s="8" t="s">
         <v>11</v>
@@ -2574,7 +2568,7 @@
         <v>63</v>
       </c>
       <c r="AQ1" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AR1" s="8" t="s">
         <v>64</v>
@@ -2589,13 +2583,13 @@
         <v>14</v>
       </c>
       <c r="AV1" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AW1" s="8" t="s">
         <v>67</v>
       </c>
       <c r="AX1" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AY1" s="8" t="s">
         <v>43</v>
@@ -2618,13 +2612,13 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -2722,13 +2716,13 @@
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -2826,13 +2820,13 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -2930,13 +2924,13 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -3040,7 +3034,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>29</v>
@@ -3144,7 +3138,7 @@
         <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
@@ -3244,7 +3238,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
@@ -3332,7 +3326,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -3420,7 +3414,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -3436,13 +3430,13 @@
         <v>71</v>
       </c>
       <c r="L10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>32</v>
@@ -3515,7 +3509,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
@@ -3532,13 +3526,13 @@
         <v>71</v>
       </c>
       <c r="L11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>77</v>
@@ -3609,16 +3603,16 @@
         <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3701,22 +3695,22 @@
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3799,22 +3793,22 @@
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3897,22 +3891,22 @@
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3995,18 +3989,18 @@
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -4099,18 +4093,18 @@
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4203,18 +4197,18 @@
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4307,18 +4301,18 @@
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -4411,28 +4405,28 @@
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I20" s="6">
         <v>25</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>71</v>
@@ -4467,7 +4461,7 @@
         <v>73</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Z20" s="2">
         <v>1200</v>
@@ -4521,28 +4515,28 @@
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I21" s="6">
         <v>25</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>71</v>
@@ -4577,7 +4571,7 @@
         <v>73</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Z21" s="2">
         <v>1</v>
@@ -4631,18 +4625,18 @@
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -4721,18 +4715,18 @@
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -4811,13 +4805,13 @@
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
@@ -4826,7 +4820,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -4836,13 +4830,13 @@
         <v>71</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M24" s="2">
-        <v>1</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O24" s="2" t="s">
         <v>32</v>
@@ -4911,13 +4905,13 @@
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -4926,7 +4920,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -4936,13 +4930,13 @@
         <v>71</v>
       </c>
       <c r="L25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M25" s="2">
-        <v>1</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>77</v>
@@ -5011,13 +5005,13 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>29</v>
@@ -5026,7 +5020,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -5109,13 +5103,13 @@
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
@@ -5124,7 +5118,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -5207,13 +5201,13 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>29</v>
@@ -5222,7 +5216,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -5305,13 +5299,13 @@
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>29</v>
@@ -5320,7 +5314,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -5403,13 +5397,13 @@
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>29</v>
@@ -5507,13 +5501,13 @@
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>29</v>
@@ -5611,13 +5605,13 @@
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>29</v>
@@ -5715,13 +5709,13 @@
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>29</v>
@@ -5819,13 +5813,13 @@
     </row>
     <row r="34" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>29</v>
@@ -5923,13 +5917,13 @@
     </row>
     <row r="35" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>29</v>
@@ -6027,13 +6021,13 @@
     </row>
     <row r="36" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>29</v>
@@ -6131,13 +6125,13 @@
     </row>
     <row r="37" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>29</v>
@@ -6237,13 +6231,13 @@
     </row>
     <row r="38" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>29</v>
@@ -6343,13 +6337,13 @@
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>29</v>
@@ -6435,13 +6429,13 @@
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>29</v>
@@ -6527,13 +6521,13 @@
     </row>
     <row r="41" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>29</v>
@@ -6627,13 +6621,13 @@
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>29</v>
@@ -6727,13 +6721,13 @@
     </row>
     <row r="43" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>29</v>
@@ -6833,13 +6827,13 @@
     </row>
     <row r="44" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>29</v>
@@ -6925,13 +6919,13 @@
     </row>
     <row r="45" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>29</v>
@@ -7025,13 +7019,13 @@
     </row>
     <row r="46" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>29</v>
@@ -7047,13 +7041,13 @@
         <v>71</v>
       </c>
       <c r="L46" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M46" s="2">
+        <v>1</v>
+      </c>
+      <c r="N46" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M46" s="2">
-        <v>1</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>32</v>
@@ -7122,13 +7116,13 @@
     </row>
     <row r="47" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>29</v>
@@ -7137,7 +7131,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -7228,13 +7222,13 @@
     </row>
     <row r="48" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>29</v>
@@ -7243,7 +7237,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -7334,13 +7328,13 @@
     </row>
     <row r="49" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>29</v>
@@ -7349,7 +7343,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -7440,13 +7434,13 @@
     </row>
     <row r="50" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>29</v>
@@ -7455,7 +7449,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -7546,13 +7540,13 @@
     </row>
     <row r="51" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>29</v>
@@ -7561,7 +7555,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -7652,13 +7646,13 @@
     </row>
     <row r="52" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>29</v>
@@ -7667,7 +7661,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -7760,13 +7754,13 @@
     </row>
     <row r="53" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>29</v>
@@ -7775,7 +7769,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -7866,13 +7860,13 @@
     </row>
     <row r="54" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>29</v>
@@ -7881,7 +7875,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -7974,13 +7968,13 @@
     </row>
     <row r="55" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>29</v>
@@ -7989,7 +7983,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -8082,13 +8076,13 @@
     </row>
     <row r="56" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>29</v>
@@ -8097,7 +8091,7 @@
         <v>2</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -8178,13 +8172,13 @@
     </row>
     <row r="57" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
@@ -8193,7 +8187,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -8274,13 +8268,13 @@
     </row>
     <row r="58" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>29</v>
@@ -8289,7 +8283,7 @@
         <v>2</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -8376,13 +8370,13 @@
     </row>
     <row r="59" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>29</v>
@@ -8391,7 +8385,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -8478,13 +8472,13 @@
     </row>
     <row r="60" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>29</v>
@@ -8493,7 +8487,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -8586,13 +8580,13 @@
     </row>
     <row r="61" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>29</v>
@@ -8601,7 +8595,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -8680,13 +8674,13 @@
     </row>
     <row r="62" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>29</v>
@@ -8695,7 +8689,7 @@
         <v>2</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -8782,13 +8776,13 @@
     </row>
     <row r="63" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>29</v>
@@ -8797,7 +8791,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -8807,13 +8801,13 @@
         <v>71</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M63" s="2">
+        <v>1</v>
+      </c>
+      <c r="N63" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M63" s="2">
-        <v>1</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>32</v>
@@ -8882,13 +8876,13 @@
     </row>
     <row r="64" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>29</v>
@@ -8986,13 +8980,13 @@
     </row>
     <row r="65" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>29</v>
@@ -9090,13 +9084,13 @@
     </row>
     <row r="66" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>29</v>
@@ -9194,13 +9188,13 @@
     </row>
     <row r="67" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>29</v>
@@ -9298,13 +9292,13 @@
     </row>
     <row r="68" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>29</v>
@@ -9402,13 +9396,13 @@
     </row>
     <row r="69" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>29</v>
@@ -9506,13 +9500,13 @@
     </row>
     <row r="70" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>29</v>
@@ -9610,13 +9604,13 @@
     </row>
     <row r="71" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>29</v>
@@ -9625,7 +9619,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -9718,13 +9712,13 @@
     </row>
     <row r="72" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>29</v>
@@ -9733,7 +9727,7 @@
         <v>2</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -9826,13 +9820,13 @@
     </row>
     <row r="73" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>29</v>
@@ -9841,7 +9835,7 @@
         <v>2</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -9926,13 +9920,13 @@
     </row>
     <row r="74" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>29</v>
@@ -9941,7 +9935,7 @@
         <v>2</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -10026,13 +10020,13 @@
     </row>
     <row r="75" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>29</v>
@@ -10041,7 +10035,7 @@
         <v>2</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -10132,13 +10126,13 @@
     </row>
     <row r="76" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>29</v>
@@ -10147,7 +10141,7 @@
         <v>2</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -10238,13 +10232,13 @@
     </row>
     <row r="77" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>29</v>
@@ -10253,7 +10247,7 @@
         <v>2</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -10346,13 +10340,13 @@
     </row>
     <row r="78" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>29</v>
@@ -10361,7 +10355,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -10440,13 +10434,13 @@
     </row>
     <row r="79" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>29</v>
@@ -10455,7 +10449,7 @@
         <v>2</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -10542,13 +10536,13 @@
     </row>
     <row r="80" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>29</v>
@@ -10557,7 +10551,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -10567,13 +10561,13 @@
         <v>71</v>
       </c>
       <c r="L80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M80" s="2">
+        <v>1</v>
+      </c>
+      <c r="N80" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M80" s="2">
-        <v>1</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O80" s="2" t="s">
         <v>32</v>
@@ -10642,13 +10636,13 @@
     </row>
     <row r="81" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>29</v>
@@ -10657,7 +10651,7 @@
         <v>2</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -10750,13 +10744,13 @@
     </row>
     <row r="82" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>29</v>
@@ -10765,7 +10759,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -10858,13 +10852,13 @@
     </row>
     <row r="83" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>29</v>
@@ -10873,7 +10867,7 @@
         <v>2</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -10964,13 +10958,13 @@
     </row>
     <row r="84" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>29</v>
@@ -10979,7 +10973,7 @@
         <v>2</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -11070,13 +11064,13 @@
     </row>
     <row r="85" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>29</v>
@@ -11085,7 +11079,7 @@
         <v>2</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -11176,13 +11170,13 @@
     </row>
     <row r="86" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>29</v>
@@ -11191,7 +11185,7 @@
         <v>2</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -11282,13 +11276,13 @@
     </row>
     <row r="87" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>29</v>
@@ -11297,7 +11291,7 @@
         <v>2</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -11388,13 +11382,13 @@
     </row>
     <row r="88" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>29</v>
@@ -11403,7 +11397,7 @@
         <v>2</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -11496,13 +11490,13 @@
     </row>
     <row r="89" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>29</v>
@@ -11511,7 +11505,7 @@
         <v>2</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -11604,13 +11598,13 @@
     </row>
     <row r="90" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>29</v>
@@ -11619,7 +11613,7 @@
         <v>2</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -11700,13 +11694,13 @@
     </row>
     <row r="91" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>29</v>
@@ -11715,7 +11709,7 @@
         <v>2</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -11796,13 +11790,13 @@
     </row>
     <row r="92" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>29</v>
@@ -11811,7 +11805,7 @@
         <v>2</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -11898,13 +11892,13 @@
     </row>
     <row r="93" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>29</v>
@@ -11913,7 +11907,7 @@
         <v>2</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -12000,13 +11994,13 @@
     </row>
     <row r="94" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>29</v>
@@ -12015,7 +12009,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -12108,13 +12102,13 @@
     </row>
     <row r="95" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>29</v>
@@ -12123,7 +12117,7 @@
         <v>2</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -12202,13 +12196,13 @@
     </row>
     <row r="96" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>29</v>
@@ -12217,7 +12211,7 @@
         <v>2</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -12304,13 +12298,13 @@
     </row>
     <row r="97" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>29</v>
@@ -12319,7 +12313,7 @@
         <v>2</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -12329,13 +12323,13 @@
         <v>71</v>
       </c>
       <c r="L97" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M97" s="2">
+        <v>1</v>
+      </c>
+      <c r="N97" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M97" s="2">
-        <v>1</v>
-      </c>
-      <c r="N97" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="O97" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
retested QA_Nitrox and Added new actions for Optimus
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DCADEE-6FEE-4849-A232-81686821DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D11D8-6BD1-43A5-9A85-CFAB835C5D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NitroXLogin" sheetId="13" r:id="rId1"/>
@@ -1252,9 +1252,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G22" sqref="G22"/>
+      <selection pane="topRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2391,9 +2391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E976D-0C3E-49F0-8D65-884140C53BC0}">
   <dimension ref="A1:BG97"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR13" sqref="AR13:AS15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3086,10 +3086,10 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AD6" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
@@ -3188,10 +3188,10 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2">
-        <v>3100</v>
+        <v>4000</v>
       </c>
       <c r="AD7" s="2">
-        <v>3900</v>
+        <v>5000</v>
       </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
@@ -3295,10 +3295,10 @@
       </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS8" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT8" s="2">
         <v>1</v>
@@ -3383,10 +3383,10 @@
       </c>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS9" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT9" s="2">
         <v>1</v>
@@ -3474,10 +3474,10 @@
       </c>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS10" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT10" s="2">
         <v>1</v>
@@ -3570,10 +3570,10 @@
       </c>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS11" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT11" s="2">
         <v>1</v>
@@ -3664,10 +3664,10 @@
       </c>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS12" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT12" s="2">
         <v>1</v>
@@ -3762,10 +3762,10 @@
       </c>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS13" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT13" s="2">
         <v>1</v>
@@ -3860,10 +3860,10 @@
       </c>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS14" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT14" s="2">
         <v>1</v>
@@ -3958,10 +3958,10 @@
       </c>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="AS15" s="2">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="AT15" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Updated the Nitrox Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D11D8-6BD1-43A5-9A85-CFAB835C5D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933B7CF7-4DBB-436C-B682-E552AEC363DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2392,8 +2392,8 @@
   <dimension ref="A1:BG97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR13" sqref="AR13:AS15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3089,7 +3089,7 @@
         <v>4000</v>
       </c>
       <c r="AD6" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
@@ -3191,7 +3191,7 @@
         <v>4000</v>
       </c>
       <c r="AD7" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
@@ -3298,7 +3298,7 @@
         <v>4000</v>
       </c>
       <c r="AS8" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT8" s="2">
         <v>1</v>
@@ -3386,7 +3386,7 @@
         <v>4000</v>
       </c>
       <c r="AS9" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT9" s="2">
         <v>1</v>
@@ -3477,7 +3477,7 @@
         <v>4000</v>
       </c>
       <c r="AS10" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT10" s="2">
         <v>1</v>
@@ -3573,7 +3573,7 @@
         <v>4000</v>
       </c>
       <c r="AS11" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT11" s="2">
         <v>1</v>
@@ -3603,7 +3603,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>169</v>
@@ -3667,7 +3667,7 @@
         <v>4000</v>
       </c>
       <c r="AS12" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT12" s="2">
         <v>1</v>
@@ -3701,7 +3701,7 @@
         <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>169</v>
@@ -3765,7 +3765,7 @@
         <v>4000</v>
       </c>
       <c r="AS13" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT13" s="2">
         <v>1</v>
@@ -3799,7 +3799,7 @@
         <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>169</v>
@@ -3863,7 +3863,7 @@
         <v>4000</v>
       </c>
       <c r="AS14" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT14" s="2">
         <v>1</v>
@@ -3897,7 +3897,7 @@
         <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>169</v>
@@ -3961,7 +3961,7 @@
         <v>4000</v>
       </c>
       <c r="AS15" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="AT15" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Updated UI Changes for Nitrox
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933B7CF7-4DBB-436C-B682-E552AEC363DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41542FC0-6662-4F94-98B2-F2117362C7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="221">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -524,9 +524,6 @@
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_077</t>
-  </si>
-  <si>
-    <t>XRP</t>
   </si>
   <si>
     <t>QA_TestCase_Auto_NitroX_079</t>
@@ -783,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -800,7 +797,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -1931,10 +1927,10 @@
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>99</v>
@@ -1976,10 +1972,10 @@
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>99</v>
@@ -2021,10 +2017,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>99</v>
@@ -2069,10 +2065,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>99</v>
@@ -2117,10 +2113,10 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>99</v>
@@ -2134,7 +2130,7 @@
       <c r="K22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="10"/>
+      <c r="L22"/>
       <c r="M22" s="9"/>
       <c r="P22" s="2">
         <v>1</v>
@@ -2164,10 +2160,10 @@
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>99</v>
@@ -2209,10 +2205,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>99</v>
@@ -2254,10 +2250,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>99</v>
@@ -2299,10 +2295,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>99</v>
@@ -2393,7 +2389,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K9" sqref="K9"/>
+      <selection pane="topRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2881,7 +2877,7 @@
         <v>3000</v>
       </c>
       <c r="AD4" s="2">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
@@ -2985,7 +2981,7 @@
         <v>3000</v>
       </c>
       <c r="AD5" s="2">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
@@ -3086,7 +3082,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AD6" s="2">
         <v>6000</v>
@@ -3188,7 +3184,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AD7" s="2">
         <v>6000</v>
@@ -3295,7 +3291,7 @@
       </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS8" s="2">
         <v>6000</v>
@@ -3383,7 +3379,7 @@
       </c>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS9" s="2">
         <v>6000</v>
@@ -3474,7 +3470,7 @@
       </c>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS10" s="2">
         <v>6000</v>
@@ -3570,7 +3566,7 @@
       </c>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS11" s="2">
         <v>6000</v>
@@ -3606,13 +3602,13 @@
         <v>109</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>169</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -3664,7 +3660,7 @@
       </c>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS12" s="2">
         <v>6000</v>
@@ -3676,10 +3672,10 @@
         <v>0.01</v>
       </c>
       <c r="AV12" s="2"/>
-      <c r="AW12" s="11">
+      <c r="AW12" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX12" s="11"/>
+      <c r="AX12" s="10"/>
       <c r="AY12" s="2" t="s">
         <v>85</v>
       </c>
@@ -3704,13 +3700,13 @@
         <v>109</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>169</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -3762,7 +3758,7 @@
       </c>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS13" s="2">
         <v>6000</v>
@@ -3774,10 +3770,10 @@
         <v>0.01</v>
       </c>
       <c r="AV13" s="2"/>
-      <c r="AW13" s="11">
+      <c r="AW13" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX13" s="11"/>
+      <c r="AX13" s="10"/>
       <c r="AY13" s="2" t="s">
         <v>85</v>
       </c>
@@ -3802,13 +3798,13 @@
         <v>109</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>169</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3860,7 +3856,7 @@
       </c>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS14" s="2">
         <v>6000</v>
@@ -3875,7 +3871,7 @@
       <c r="AW14" s="7">
         <v>28</v>
       </c>
-      <c r="AX14" s="11"/>
+      <c r="AX14" s="10"/>
       <c r="AY14" s="2" t="s">
         <v>85</v>
       </c>
@@ -3900,13 +3896,13 @@
         <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>169</v>
+        <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3958,7 +3954,7 @@
       </c>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="AS15" s="2">
         <v>6000</v>
@@ -3970,10 +3966,10 @@
         <v>0.01</v>
       </c>
       <c r="AV15" s="2"/>
-      <c r="AW15" s="12">
+      <c r="AW15" s="11">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX15" s="12"/>
+      <c r="AX15" s="11"/>
       <c r="AY15" s="2" t="s">
         <v>85</v>
       </c>
@@ -3989,18 +3985,18 @@
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -4093,18 +4089,18 @@
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -4197,18 +4193,18 @@
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -4301,18 +4297,18 @@
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -4411,12 +4407,12 @@
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
@@ -4521,12 +4517,12 @@
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -4631,12 +4627,12 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -4721,12 +4717,12 @@
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -4811,7 +4807,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
@@ -4820,7 +4816,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -4911,7 +4907,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -4920,7 +4916,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -5005,13 +5001,13 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>29</v>
@@ -5020,7 +5016,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -5084,10 +5080,10 @@
         <v>0.01</v>
       </c>
       <c r="AV26" s="2"/>
-      <c r="AW26" s="11">
+      <c r="AW26" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX26" s="11"/>
+      <c r="AX26" s="10"/>
       <c r="AY26" s="2" t="s">
         <v>85</v>
       </c>
@@ -5103,13 +5099,13 @@
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
@@ -5118,7 +5114,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -5182,10 +5178,10 @@
         <v>0.01</v>
       </c>
       <c r="AV27" s="2"/>
-      <c r="AW27" s="11">
+      <c r="AW27" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX27" s="11"/>
+      <c r="AX27" s="10"/>
       <c r="AY27" s="2" t="s">
         <v>85</v>
       </c>
@@ -5201,13 +5197,13 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>29</v>
@@ -5216,7 +5212,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -5280,10 +5276,10 @@
         <v>0.01</v>
       </c>
       <c r="AV28" s="2"/>
-      <c r="AW28" s="11">
+      <c r="AW28" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX28" s="11"/>
+      <c r="AX28" s="10"/>
       <c r="AY28" s="2" t="s">
         <v>85</v>
       </c>
@@ -5299,13 +5295,13 @@
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>29</v>
@@ -5314,7 +5310,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -5378,10 +5374,10 @@
         <v>0.01</v>
       </c>
       <c r="AV29" s="2"/>
-      <c r="AW29" s="11">
+      <c r="AW29" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX29" s="11"/>
+      <c r="AX29" s="10"/>
       <c r="AY29" s="2" t="s">
         <v>85</v>
       </c>
@@ -6600,10 +6596,10 @@
         <v>0.01</v>
       </c>
       <c r="AV41" s="2"/>
-      <c r="AW41" s="11">
+      <c r="AW41" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX41" s="11">
+      <c r="AX41" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY41" s="2" t="s">
@@ -6621,7 +6617,7 @@
     </row>
     <row r="42" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>85</v>
@@ -6700,10 +6696,10 @@
         <v>0.01</v>
       </c>
       <c r="AV42" s="2"/>
-      <c r="AW42" s="11">
+      <c r="AW42" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX42" s="11">
+      <c r="AX42" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY42" s="2" t="s">
@@ -6998,10 +6994,10 @@
         <v>0.01</v>
       </c>
       <c r="AV45" s="2"/>
-      <c r="AW45" s="11">
+      <c r="AW45" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX45" s="11">
+      <c r="AX45" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY45" s="2" t="s">
@@ -7122,7 +7118,7 @@
         <v>23</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>29</v>
@@ -7131,7 +7127,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -7228,7 +7224,7 @@
         <v>23</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>29</v>
@@ -7237,7 +7233,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -7334,7 +7330,7 @@
         <v>23</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>29</v>
@@ -7343,7 +7339,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -7434,13 +7430,13 @@
     </row>
     <row r="50" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>29</v>
@@ -7449,7 +7445,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -7546,7 +7542,7 @@
         <v>23</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>29</v>
@@ -7555,7 +7551,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -7646,13 +7642,13 @@
     </row>
     <row r="52" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>29</v>
@@ -7661,7 +7657,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -7754,13 +7750,13 @@
     </row>
     <row r="53" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>29</v>
@@ -7769,7 +7765,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -7860,13 +7856,13 @@
     </row>
     <row r="54" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>29</v>
@@ -7875,7 +7871,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -7968,13 +7964,13 @@
     </row>
     <row r="55" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>29</v>
@@ -7983,7 +7979,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -8076,13 +8072,13 @@
     </row>
     <row r="56" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>29</v>
@@ -8091,7 +8087,7 @@
         <v>2</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -8172,13 +8168,13 @@
     </row>
     <row r="57" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
@@ -8187,7 +8183,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -8268,13 +8264,13 @@
     </row>
     <row r="58" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>29</v>
@@ -8283,7 +8279,7 @@
         <v>2</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -8349,10 +8345,10 @@
         <v>0.01</v>
       </c>
       <c r="AV58" s="2"/>
-      <c r="AW58" s="11">
+      <c r="AW58" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX58" s="11">
+      <c r="AX58" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY58" s="2" t="s">
@@ -8370,13 +8366,13 @@
     </row>
     <row r="59" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>29</v>
@@ -8385,7 +8381,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -8451,10 +8447,10 @@
         <v>0.01</v>
       </c>
       <c r="AV59" s="2"/>
-      <c r="AW59" s="11">
+      <c r="AW59" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX59" s="11">
+      <c r="AX59" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY59" s="2" t="s">
@@ -8472,13 +8468,13 @@
     </row>
     <row r="60" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>29</v>
@@ -8487,7 +8483,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -8580,13 +8576,13 @@
     </row>
     <row r="61" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>29</v>
@@ -8595,7 +8591,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -8674,13 +8670,13 @@
     </row>
     <row r="62" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>29</v>
@@ -8689,7 +8685,7 @@
         <v>2</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -8755,10 +8751,10 @@
         <v>0.01</v>
       </c>
       <c r="AV62" s="2"/>
-      <c r="AW62" s="11">
+      <c r="AW62" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX62" s="11">
+      <c r="AX62" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY62" s="2" t="s">
@@ -8776,13 +8772,13 @@
     </row>
     <row r="63" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>29</v>
@@ -8791,7 +8787,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -9604,13 +9600,13 @@
     </row>
     <row r="71" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>29</v>
@@ -9619,7 +9615,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -9712,13 +9708,13 @@
     </row>
     <row r="72" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>29</v>
@@ -9727,7 +9723,7 @@
         <v>2</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -9820,13 +9816,13 @@
     </row>
     <row r="73" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>29</v>
@@ -9835,7 +9831,7 @@
         <v>2</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -9920,13 +9916,13 @@
     </row>
     <row r="74" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>29</v>
@@ -9935,7 +9931,7 @@
         <v>2</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -10020,13 +10016,13 @@
     </row>
     <row r="75" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>29</v>
@@ -10035,7 +10031,7 @@
         <v>2</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -10105,10 +10101,10 @@
         <v>0.01</v>
       </c>
       <c r="AV75" s="2"/>
-      <c r="AW75" s="11">
+      <c r="AW75" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX75" s="11">
+      <c r="AX75" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY75" s="2" t="s">
@@ -10126,13 +10122,13 @@
     </row>
     <row r="76" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>29</v>
@@ -10141,7 +10137,7 @@
         <v>2</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -10211,10 +10207,10 @@
         <v>0.01</v>
       </c>
       <c r="AV76" s="2"/>
-      <c r="AW76" s="11">
+      <c r="AW76" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX76" s="11">
+      <c r="AX76" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY76" s="2" t="s">
@@ -10232,13 +10228,13 @@
     </row>
     <row r="77" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>29</v>
@@ -10247,7 +10243,7 @@
         <v>2</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -10340,13 +10336,13 @@
     </row>
     <row r="78" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>29</v>
@@ -10355,7 +10351,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -10434,13 +10430,13 @@
     </row>
     <row r="79" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>29</v>
@@ -10449,7 +10445,7 @@
         <v>2</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -10515,10 +10511,10 @@
         <v>0.01</v>
       </c>
       <c r="AV79" s="2"/>
-      <c r="AW79" s="11">
+      <c r="AW79" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX79" s="11">
+      <c r="AX79" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY79" s="2" t="s">
@@ -10536,13 +10532,13 @@
     </row>
     <row r="80" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>29</v>
@@ -10551,7 +10547,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -10636,13 +10632,13 @@
     </row>
     <row r="81" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>29</v>
@@ -10651,7 +10647,7 @@
         <v>2</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -10744,13 +10740,13 @@
     </row>
     <row r="82" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>29</v>
@@ -10759,7 +10755,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -10852,13 +10848,13 @@
     </row>
     <row r="83" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>29</v>
@@ -10867,7 +10863,7 @@
         <v>2</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -10958,13 +10954,13 @@
     </row>
     <row r="84" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>29</v>
@@ -10973,7 +10969,7 @@
         <v>2</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -11064,13 +11060,13 @@
     </row>
     <row r="85" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>29</v>
@@ -11079,7 +11075,7 @@
         <v>2</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -11170,13 +11166,13 @@
     </row>
     <row r="86" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>29</v>
@@ -11185,7 +11181,7 @@
         <v>2</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -11276,13 +11272,13 @@
     </row>
     <row r="87" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>29</v>
@@ -11291,7 +11287,7 @@
         <v>2</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -11382,13 +11378,13 @@
     </row>
     <row r="88" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>29</v>
@@ -11397,7 +11393,7 @@
         <v>2</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -11490,13 +11486,13 @@
     </row>
     <row r="89" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>29</v>
@@ -11505,7 +11501,7 @@
         <v>2</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -11598,13 +11594,13 @@
     </row>
     <row r="90" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>29</v>
@@ -11613,7 +11609,7 @@
         <v>2</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -11694,13 +11690,13 @@
     </row>
     <row r="91" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>29</v>
@@ -11709,7 +11705,7 @@
         <v>2</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -11790,13 +11786,13 @@
     </row>
     <row r="92" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>29</v>
@@ -11805,7 +11801,7 @@
         <v>2</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -11871,10 +11867,10 @@
         <v>0.01</v>
       </c>
       <c r="AV92" s="2"/>
-      <c r="AW92" s="11">
+      <c r="AW92" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX92" s="11">
+      <c r="AX92" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY92" s="2" t="s">
@@ -11892,13 +11888,13 @@
     </row>
     <row r="93" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>29</v>
@@ -11907,7 +11903,7 @@
         <v>2</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -11973,10 +11969,10 @@
         <v>0.01</v>
       </c>
       <c r="AV93" s="2"/>
-      <c r="AW93" s="11">
+      <c r="AW93" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX93" s="11">
+      <c r="AX93" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY93" s="2" t="s">
@@ -11994,13 +11990,13 @@
     </row>
     <row r="94" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>29</v>
@@ -12009,7 +12005,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -12102,13 +12098,13 @@
     </row>
     <row r="95" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>29</v>
@@ -12117,7 +12113,7 @@
         <v>2</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -12196,13 +12192,13 @@
     </row>
     <row r="96" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>29</v>
@@ -12211,7 +12207,7 @@
         <v>2</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -12277,10 +12273,10 @@
         <v>0.01</v>
       </c>
       <c r="AV96" s="2"/>
-      <c r="AW96" s="11">
+      <c r="AW96" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AX96" s="11">
+      <c r="AX96" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY96" s="2" t="s">
@@ -12298,13 +12294,13 @@
     </row>
     <row r="97" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>29</v>
@@ -12313,7 +12309,7 @@
         <v>2</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>

</xml_diff>

<commit_message>
Optimized NitroX and UI Chnages
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/NitroX.xlsx
+++ b/src/test/resources/testData/NitroX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41542FC0-6662-4F94-98B2-F2117362C7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D087C-89DE-4AE8-BF84-270B6406C83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1248,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763A6C0-A0DE-42F1-A4CC-B0EEDE6F7213}">
   <dimension ref="A1:XFC34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
     </sheetView>
@@ -2388,8 +2388,8 @@
   <dimension ref="A1:BG97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AY10" sqref="AY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>